<commit_message>
create patients feature file
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\CasesUpdate\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47ABC11D-0080-42EE-98DA-1A3CAF17AAFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0529F6-9B41-4E10-8606-FD6A18814BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
@@ -398,7 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>

</xml_diff>

<commit_message>
Add consent details to person accounts
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\CasesUpdate\pep-automation\src\main\java\config\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\TestData\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0529F6-9B41-4E10-8606-FD6A18814BB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5AF0BE-36E6-458D-B811-945FCFED0595}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
@@ -398,9 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>

</xml_diff>

<commit_message>
Adding Code For Payer Operation Part_1
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\CasesUpdate\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,15 +33,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>PatientID</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009515</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -396,13 +400,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
@@ -410,6 +414,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Code For Payer Insurance Creation
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\TestData\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,15 +33,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>PatientID</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009581</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009582</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009583</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009584</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009589</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009594</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009599</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009602</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009603</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009604</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009605</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009606</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009607</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009609</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009611</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009612</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009630</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009631</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009632</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009633</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009642</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009643</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009647</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009648</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009649</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009650</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009651</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -396,13 +478,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
@@ -410,6 +492,141 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding Comments and N_A handdle for Payer
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>PatientID</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>PEP_ID-2009651</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009652</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009655</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009656</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -627,6 +636,21 @@
         <v>27</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Create testData flow update
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\TestRefactor\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78233947-B66B-4DC2-91F1-174FB4C7C32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D786F9-F9BC-4D43-A68A-024F25A03A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1090" windowWidth="19200" windowHeight="5100" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="pepID" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>

</xml_diff>

<commit_message>
create care team member update
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\TestRefactor\pep-automation\src\main\java\config\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D786F9-F9BC-4D43-A68A-024F25A03A12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C812506-08EA-4B63-B80F-9F9817E0CEDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
remove reflection login steps
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kjbj453\Documents\TestRefactor\pep-automation\src\main\java\config\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjbj453/executeRegressionReflection/pep-automation/src/main/java/config/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C812506-08EA-4B63-B80F-9F9817E0CEDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609503EA-61FB-C247-8400-093166F6F076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="pepID" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,58 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>PatientID</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PEP_ID-2011148</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011149</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011151</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011152</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011153</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011154</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011155</t>
-  </si>
-  <si>
-    <t>PEP_ID-2011156</t>
-  </si>
-  <si>
-    <t>PEP_ID-2004071</t>
-  </si>
-  <si>
-    <t>PEP_ID-2004072</t>
-  </si>
-  <si>
-    <t>PEP_ID-2004077</t>
-  </si>
-  <si>
-    <t>PEP_ID-2004078</t>
-  </si>
-  <si>
-    <t>PEP_ID-2004080</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -439,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.36328125" collapsed="true"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
@@ -455,76 +412,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor_6 Maintenance for Patients.feature
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>PatientID</t>
   </si>
@@ -78,6 +78,75 @@
   </si>
   <si>
     <t>PEP_ID-2004080</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005243</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005248</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005250</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005275</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005396</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005410</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005419</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005424</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005427</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005478</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005485</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005493</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005559</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005562</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005568</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005585</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005588</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005591</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005596</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005603</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005607</t>
+  </si>
+  <si>
+    <t>PEP_ID-2005609</t>
   </si>
 </sst>
 </file>
@@ -439,7 +508,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -525,6 +594,136 @@
         <v>14</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
remove reflection and fix smoke scenarios
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjbj453/executeRegressionReflection/pep-automation/src/main/java/config/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F45263-6C1E-BD4E-AA01-DD5489D49666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66B7175-D924-DB4F-9719-6957D8B189A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19420" windowHeight="10420" xr2:uid="{ECF7F460-8D37-4829-BDD8-96C40B84DA4A}"/>
   </bookViews>
@@ -398,9 +398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Refactor_8 remove code hardcode
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjbj453/executeRegressionReflection/pep-automation/src/main/java/config/excel/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,15 +33,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>PatientID</t>
+  </si>
+  <si>
+    <t>PEP_ID-2006019</t>
+  </si>
+  <si>
+    <t>PEP_ID-2006022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -396,13 +403,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
@@ -410,6 +417,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor_8 adding import class Values to login page
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>PatientID</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>PEP_ID-2006022</t>
+  </si>
+  <si>
+    <t>PEP_ID-2006173</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -427,6 +430,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding the class SendEmail to send report
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>PatientID</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>PEP_ID-2007251</t>
+  </si>
+  <si>
+    <t>PEP_ID-2007800</t>
+  </si>
+  <si>
+    <t>PEP_ID-2007802</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -451,6 +457,16 @@
         <v>5</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixes For July Sanity
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>PatientID</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>PEP_ID-2007802</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009237</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009241</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009243</t>
   </si>
 </sst>
 </file>
@@ -418,7 +427,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -467,6 +476,21 @@
         <v>7</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
PatientDataCreation.feature Fixed, Iframe Changes
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>PatientID</t>
   </si>
@@ -66,6 +66,57 @@
   </si>
   <si>
     <t>PEP_ID-2009243</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009336</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009337</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009338</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009339</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009340</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009342</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009343</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009344</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009347</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009349</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009350</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009351</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009352</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009353</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009354</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009357</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009358</t>
   </si>
 </sst>
 </file>
@@ -427,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -491,6 +542,91 @@
         <v>10</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enhance of method switching frame
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>PatientID</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>PEP_ID-2009358</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009386</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009388</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009389</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009391</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009392</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009393</t>
   </si>
 </sst>
 </file>
@@ -478,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -627,6 +645,36 @@
         <v>27</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Email Update easier configuration.
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>PatientID</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>PEP_ID-2009434</t>
+  </si>
+  <si>
+    <t>PEP_ID-2009435</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A38"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -707,6 +710,11 @@
         <v>37</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update patient creation flow
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjbj453/RefactorPatients/pep-automation/src/main/java/config/excel/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,15 +33,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>PatientID</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>PEP_ID-2010444</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -396,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -404,7 +411,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="18">
@@ -412,6 +419,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Product Master issue Fix PE search
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="3">
   <si>
     <t>PatientID</t>
   </si>
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A153"/>
+  <dimension ref="A1:A163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1179,6 +1179,56 @@
         <v>1</v>
       </c>
     </row>
+    <row r="154">
+      <c r="A154" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix To SPP Creation adding first the Consents
</commit_message>
<xml_diff>
--- a/src/main/java/config/excel/patientList.xlsx
+++ b/src/main/java/config/excel/patientList.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="3">
   <si>
     <t>PatientID</t>
   </si>
@@ -403,7 +403,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4E02AE-7D8D-4925-8A0E-088D68878E9C}">
-  <dimension ref="A1:A163"/>
+  <dimension ref="A1:A176"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1229,6 +1229,71 @@
         <v>1</v>
       </c>
     </row>
+    <row r="164">
+      <c r="A164" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>